<commit_message>
fix gráficos de respostas do forms
</commit_message>
<xml_diff>
--- a/Pesquisa de requisitos/StackTec (respostas).xlsx
+++ b/Pesquisa de requisitos/StackTec (respostas).xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ieca\OneDrive - GFT Technologies SE\Documents\facul\ES2N_Guaxinim_Raivoso\Pesquisa de requisitos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269090FC-CDF8-4A9C-8AED-85F8FF7B0408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Respostas ao formulário" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Gráficos" sheetId="2" r:id="rId5"/>
+    <sheet name="Respostas ao formulário" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -686,18 +694,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -708,107 +717,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6267450" cy="2790825"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6953250" cy="3152775"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -998,28 +945,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="18.88"/>
-    <col customWidth="1" min="4" max="4" width="9.38"/>
-    <col customWidth="1" min="5" max="24" width="18.88"/>
+    <col min="1" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="24" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1075,9 +1025,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44647.80954087963</v>
+        <v>44647.809540879629</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
@@ -1122,10 +1072,10 @@
         <v>25</v>
       </c>
       <c r="P2" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44647.811740289355</v>
       </c>
@@ -1172,10 +1122,10 @@
         <v>25</v>
       </c>
       <c r="P3" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44647.812815578705</v>
       </c>
@@ -1219,7 +1169,7 @@
         <v>25</v>
       </c>
       <c r="P4" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>39</v>
@@ -1228,7 +1178,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44647.81287627315</v>
       </c>
@@ -1272,15 +1222,15 @@
         <v>25</v>
       </c>
       <c r="P5" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44647.8128769676</v>
+        <v>44647.812876967597</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>47</v>
@@ -1325,10 +1275,10 @@
         <v>25</v>
       </c>
       <c r="P6" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44647.813794456015</v>
       </c>
@@ -1375,15 +1325,15 @@
         <v>25</v>
       </c>
       <c r="P7" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44647.81616636574</v>
+        <v>44647.816166365737</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>57</v>
@@ -1425,15 +1375,15 @@
         <v>25</v>
       </c>
       <c r="P8" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44647.81977594907</v>
+        <v>44647.819775949072</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>62</v>
@@ -1478,7 +1428,7 @@
         <v>25</v>
       </c>
       <c r="P9" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>66</v>
@@ -1487,7 +1437,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44647.81996403935</v>
       </c>
@@ -1534,15 +1484,15 @@
         <v>25</v>
       </c>
       <c r="P10" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44647.82163424768</v>
+        <v>44647.821634247681</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>73</v>
@@ -1587,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="P11" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>77</v>
@@ -1596,9 +1546,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44647.82178090278</v>
+        <v>44647.821780902777</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>79</v>
@@ -1643,15 +1593,15 @@
         <v>25</v>
       </c>
       <c r="P12" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44647.82192890046</v>
+        <v>44647.821928900463</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>83</v>
@@ -1696,7 +1646,7 @@
         <v>25</v>
       </c>
       <c r="P13" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>86</v>
@@ -1705,7 +1655,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44647.828744363425</v>
       </c>
@@ -1752,7 +1702,7 @@
         <v>90</v>
       </c>
       <c r="P14" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>91</v>
@@ -1761,7 +1711,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44647.829312546295</v>
       </c>
@@ -1808,7 +1758,7 @@
         <v>25</v>
       </c>
       <c r="P15" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>96</v>
@@ -1817,9 +1767,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44647.8369968287</v>
+        <v>44647.836996828701</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>98</v>
@@ -1864,7 +1814,7 @@
         <v>25</v>
       </c>
       <c r="P16" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>101</v>
@@ -1873,9 +1823,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44647.84243222223</v>
+        <v>44647.842432222227</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>103</v>
@@ -1920,7 +1870,7 @@
         <v>25</v>
       </c>
       <c r="P17" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>107</v>
@@ -1929,7 +1879,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44647.85677888889</v>
       </c>
@@ -1976,13 +1926,13 @@
         <v>25</v>
       </c>
       <c r="P18" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44647.857436481485</v>
       </c>
@@ -2023,13 +1973,13 @@
         <v>25</v>
       </c>
       <c r="P19" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44647.859427187504</v>
       </c>
@@ -2076,7 +2026,7 @@
         <v>25</v>
       </c>
       <c r="P20" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>118</v>
@@ -2085,9 +2035,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44647.86369950231</v>
+        <v>44647.863699502312</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>120</v>
@@ -2132,7 +2082,7 @@
         <v>25</v>
       </c>
       <c r="P21" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>123</v>
@@ -2141,9 +2091,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44647.89216271991</v>
+        <v>44647.892162719909</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>125</v>
@@ -2188,15 +2138,15 @@
         <v>90</v>
       </c>
       <c r="P22" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44647.89440567129</v>
+        <v>44647.894405671293</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>129</v>
@@ -2238,10 +2188,10 @@
         <v>38</v>
       </c>
       <c r="P23" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44647.89532585648</v>
       </c>
@@ -2288,7 +2238,7 @@
         <v>25</v>
       </c>
       <c r="P24" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>134</v>
@@ -2297,9 +2247,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44647.90447043981</v>
+        <v>44647.904470439811</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>136</v>
@@ -2341,10 +2291,10 @@
         <v>25</v>
       </c>
       <c r="P25" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44647.92118907407</v>
       </c>
@@ -2391,12 +2341,12 @@
         <v>25</v>
       </c>
       <c r="P26" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44647.9298569213</v>
+        <v>44647.929856921299</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>143</v>
@@ -2441,10 +2391,10 @@
         <v>25</v>
       </c>
       <c r="P27" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44647.935174293976</v>
       </c>
@@ -2491,10 +2441,10 @@
         <v>25</v>
       </c>
       <c r="P28" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44647.93883741898</v>
       </c>
@@ -2541,15 +2491,15 @@
         <v>25</v>
       </c>
       <c r="P29" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q29" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44647.9441422338</v>
+        <v>44647.944142233799</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>153</v>
@@ -2591,12 +2541,12 @@
         <v>25</v>
       </c>
       <c r="P30" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44647.9501716088</v>
+        <v>44647.950171608798</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>154</v>
@@ -2638,15 +2588,15 @@
         <v>25</v>
       </c>
       <c r="P31" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44647.97601612269</v>
+        <v>44647.976016122688</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>156</v>
@@ -2688,10 +2638,10 @@
         <v>25</v>
       </c>
       <c r="P32" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44647.987316087965</v>
       </c>
@@ -2738,12 +2688,12 @@
         <v>25</v>
       </c>
       <c r="P33" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44647.98902454861</v>
+        <v>44647.989024548609</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>161</v>
@@ -2788,7 +2738,7 @@
         <v>25</v>
       </c>
       <c r="P34" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>164</v>
@@ -2797,9 +2747,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>44648.00242596064</v>
+        <v>44648.002425960643</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>166</v>
@@ -2844,13 +2794,13 @@
         <v>25</v>
       </c>
       <c r="P35" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44648.259067418985</v>
       </c>
@@ -2897,7 +2847,7 @@
         <v>25</v>
       </c>
       <c r="P36" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>174</v>
@@ -2906,7 +2856,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44648.327630451386</v>
       </c>
@@ -2953,7 +2903,7 @@
         <v>25</v>
       </c>
       <c r="P37" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>177</v>
@@ -2962,9 +2912,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44648.41529783564</v>
+        <v>44648.415297835643</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>178</v>
@@ -3009,7 +2959,7 @@
         <v>25</v>
       </c>
       <c r="P38" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q38" s="3" t="s">
         <v>182</v>
@@ -3018,9 +2968,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44648.42290172454</v>
+        <v>44648.422901724538</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>184</v>
@@ -3065,7 +3015,7 @@
         <v>25</v>
       </c>
       <c r="P39" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>186</v>
@@ -3074,9 +3024,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44648.43229982639</v>
+        <v>44648.432299826389</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>188</v>
@@ -3121,7 +3071,7 @@
         <v>25</v>
       </c>
       <c r="P40" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>191</v>
@@ -3130,9 +3080,9 @@
         <v>192</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44648.53718164352</v>
+        <v>44648.537181643522</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>193</v>
@@ -3177,15 +3127,15 @@
         <v>25</v>
       </c>
       <c r="P41" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44648.56358336806</v>
+        <v>44648.563583368057</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>196</v>
@@ -3230,7 +3180,7 @@
         <v>25</v>
       </c>
       <c r="P42" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>199</v>
@@ -3239,9 +3189,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44648.79448755787</v>
+        <v>44648.794487557869</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>201</v>
@@ -3286,13 +3236,13 @@
         <v>25</v>
       </c>
       <c r="P43" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44649.30336539352</v>
       </c>
@@ -3339,12 +3289,12 @@
         <v>25</v>
       </c>
       <c r="P44" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44649.62440003472</v>
+        <v>44649.624400034721</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>208</v>
@@ -3389,15 +3339,15 @@
         <v>25</v>
       </c>
       <c r="P45" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44649.69851354166</v>
+        <v>44649.698513541662</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>211</v>
@@ -3442,15 +3392,15 @@
         <v>25</v>
       </c>
       <c r="P46" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44650.49806087963</v>
+        <v>44650.498060879632</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>214</v>
@@ -3495,7 +3445,7 @@
         <v>25</v>
       </c>
       <c r="P47" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>217</v>
@@ -3504,9 +3454,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44654.79574563657</v>
+        <v>44654.795745636569</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>219</v>
@@ -3551,7 +3501,7 @@
         <v>25</v>
       </c>
       <c r="P48" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>221</v>
@@ -3561,66 +3511,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="10">
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11">
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12">
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13">
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="4"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>